<commit_message>
Load Data from xlse file suffle all questions and make 20 questions Get data and print it test_largepart.html make question <div> 'alloctated'
</commit_message>
<xml_diff>
--- a/datafiles/questionDB.xlsx
+++ b/datafiles/questionDB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songi/Desktop/MyProjects/TestMaker/datafiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{20B0E479-3FD6-3F42-8E5C-80485BAD1AEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF46D53E-F886-844B-A767-B15BD8DB64D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14400" yWindow="500" windowWidth="14400" windowHeight="17500" xr2:uid="{0D182CA0-F053-8B46-8287-4831F5560F7B}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="63">
   <si>
     <t>name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -276,197 +276,18 @@
     <t>http://www.jkmeat.co.kr/skin_shop/standard/s_img/basic/JK-0424_M.jpg</t>
   </si>
   <si>
-    <t>http://www.jkmeat.co.kr/skin_shop/standard/s_img/basic/JK-0425_M.jpg</t>
-  </si>
-  <si>
-    <t>http://www.jkmeat.co.kr/skin_shop/standard/s_img/basic/JK-0426_M.jpg</t>
-  </si>
-  <si>
-    <t>http://www.jkmeat.co.kr/skin_shop/standard/s_img/basic/JK-0427_M.jpg</t>
-  </si>
-  <si>
-    <t>http://www.jkmeat.co.kr/skin_shop/standard/s_img/basic/JK-0428_M.jpg</t>
-  </si>
-  <si>
-    <t>http://www.jkmeat.co.kr/skin_shop/standard/s_img/basic/JK-0429_M.jpg</t>
-  </si>
-  <si>
-    <t>http://www.jkmeat.co.kr/skin_shop/standard/s_img/basic/JK-0430_M.jpg</t>
-  </si>
-  <si>
-    <t>http://www.jkmeat.co.kr/skin_shop/standard/s_img/basic/JK-0431_M.jpg</t>
-  </si>
-  <si>
-    <t>http://www.jkmeat.co.kr/skin_shop/standard/s_img/basic/JK-0432_M.jpg</t>
-  </si>
-  <si>
-    <t>http://www.jkmeat.co.kr/skin_shop/standard/s_img/basic/JK-0433_M.jpg</t>
-  </si>
-  <si>
-    <t>http://www.jkmeat.co.kr/skin_shop/standard/s_img/basic/JK-0434_M.jpg</t>
-  </si>
-  <si>
-    <t>http://www.jkmeat.co.kr/skin_shop/standard/s_img/basic/JK-0435_M.jpg</t>
-  </si>
-  <si>
-    <t>http://www.jkmeat.co.kr/skin_shop/standard/s_img/basic/JK-0436_M.jpg</t>
-  </si>
-  <si>
-    <t>http://www.jkmeat.co.kr/skin_shop/standard/s_img/basic/JK-0437_M.jpg</t>
-  </si>
-  <si>
-    <t>http://www.jkmeat.co.kr/skin_shop/standard/s_img/basic/JK-0438_M.jpg</t>
-  </si>
-  <si>
-    <t>http://www.jkmeat.co.kr/skin_shop/standard/s_img/basic/JK-0439_M.jpg</t>
-  </si>
-  <si>
-    <t>http://www.jkmeat.co.kr/skin_shop/standard/s_img/basic/JK-0440_M.jpg</t>
-  </si>
-  <si>
-    <t>http://www.jkmeat.co.kr/skin_shop/standard/s_img/basic/JK-0441_M.jpg</t>
-  </si>
-  <si>
-    <t>http://www.jkmeat.co.kr/skin_shop/standard/s_img/basic/JK-0442_M.jpg</t>
-  </si>
-  <si>
-    <t>http://www.jkmeat.co.kr/skin_shop/standard/s_img/basic/JK-0443_M.jpg</t>
-  </si>
-  <si>
-    <t>http://www.jkmeat.co.kr/skin_shop/standard/s_img/basic/JK-0444_M.jpg</t>
-  </si>
-  <si>
-    <t>http://www.jkmeat.co.kr/skin_shop/standard/s_img/basic/JK-0445_M.jpg</t>
-  </si>
-  <si>
-    <t>http://www.jkmeat.co.kr/skin_shop/standard/s_img/basic/JK-0446_M.jpg</t>
-  </si>
-  <si>
-    <t>http://www.jkmeat.co.kr/skin_shop/standard/s_img/basic/JK-0447_M.jpg</t>
-  </si>
-  <si>
     <t>http://image.auction.co.kr/itemimage/1f/02/25/1f02252136.jpg</t>
   </si>
   <si>
-    <t>http://image.auction.co.kr/itemimage/1f/02/25/1f02252137.jpg</t>
-  </si>
-  <si>
-    <t>http://image.auction.co.kr/itemimage/1f/02/25/1f02252138.jpg</t>
-  </si>
-  <si>
-    <t>http://image.auction.co.kr/itemimage/1f/02/25/1f02252139.jpg</t>
-  </si>
-  <si>
-    <t>http://image.auction.co.kr/itemimage/1f/02/25/1f02252140.jpg</t>
-  </si>
-  <si>
-    <t>http://image.auction.co.kr/itemimage/1f/02/25/1f02252141.jpg</t>
-  </si>
-  <si>
-    <t>http://image.auction.co.kr/itemimage/1f/02/25/1f02252142.jpg</t>
-  </si>
-  <si>
-    <t>http://image.auction.co.kr/itemimage/1f/02/25/1f02252143.jpg</t>
-  </si>
-  <si>
-    <t>http://image.auction.co.kr/itemimage/1f/02/25/1f02252144.jpg</t>
-  </si>
-  <si>
-    <t>http://image.auction.co.kr/itemimage/1f/02/25/1f02252145.jpg</t>
-  </si>
-  <si>
-    <t>http://image.auction.co.kr/itemimage/1f/02/25/1f02252146.jpg</t>
-  </si>
-  <si>
-    <t>http://image.auction.co.kr/itemimage/1f/02/25/1f02252147.jpg</t>
-  </si>
-  <si>
-    <t>http://image.auction.co.kr/itemimage/1f/02/25/1f02252148.jpg</t>
-  </si>
-  <si>
-    <t>http://image.auction.co.kr/itemimage/1f/02/25/1f02252149.jpg</t>
-  </si>
-  <si>
-    <t>http://image.auction.co.kr/itemimage/1f/02/25/1f02252150.jpg</t>
-  </si>
-  <si>
-    <t>http://image.auction.co.kr/itemimage/1f/02/25/1f02252151.jpg</t>
-  </si>
-  <si>
-    <t>http://image.auction.co.kr/itemimage/1f/02/25/1f02252152.jpg</t>
-  </si>
-  <si>
-    <t>http://image.auction.co.kr/itemimage/1f/02/25/1f02252153.jpg</t>
-  </si>
-  <si>
-    <t>http://image.auction.co.kr/itemimage/1f/02/25/1f02252154.jpg</t>
-  </si>
-  <si>
-    <t>http://image.auction.co.kr/itemimage/1f/02/25/1f02252155.jpg</t>
-  </si>
-  <si>
-    <t>http://image.auction.co.kr/itemimage/1f/02/25/1f02252156.jpg</t>
-  </si>
-  <si>
-    <t>http://image.auction.co.kr/itemimage/1f/02/25/1f02252157.jpg</t>
-  </si>
-  <si>
-    <t>http://image.auction.co.kr/itemimage/1f/02/25/1f02252158.jpg</t>
-  </si>
-  <si>
-    <t>http://image.auction.co.kr/itemimage/1f/02/25/1f02252159.jpg</t>
-  </si>
-  <si>
-    <t>http://image.auction.co.kr/itemimage/1f/02/25/1f02252160.jpg</t>
-  </si>
-  <si>
-    <t>http://image.auction.co.kr/itemimage/1f/02/25/1f02252161.jpg</t>
-  </si>
-  <si>
-    <t>http://image.auction.co.kr/itemimage/1f/02/25/1f02252162.jpg</t>
-  </si>
-  <si>
-    <t>http://image.auction.co.kr/itemimage/1f/02/25/1f02252163.jpg</t>
-  </si>
-  <si>
-    <t>http://image.auction.co.kr/itemimage/1f/02/25/1f02252164.jpg</t>
-  </si>
-  <si>
-    <t>http://image.auction.co.kr/itemimage/1f/02/25/1f02252165.jpg</t>
-  </si>
-  <si>
-    <t>http://image.auction.co.kr/itemimage/1f/02/25/1f02252166.jpg</t>
-  </si>
-  <si>
-    <t>http://image.auction.co.kr/itemimage/1f/02/25/1f02252167.jpg</t>
-  </si>
-  <si>
-    <t>http://image.auction.co.kr/itemimage/1f/02/25/1f02252168.jpg</t>
-  </si>
-  <si>
-    <t>http://image.auction.co.kr/itemimage/1f/02/25/1f02252169.jpg</t>
-  </si>
-  <si>
-    <t>http://image.auction.co.kr/itemimage/1f/02/25/1f02252170.jpg</t>
-  </si>
-  <si>
-    <t>http://image.auction.co.kr/itemimage/1f/02/25/1f02252171.jpg</t>
-  </si>
-  <si>
-    <t>http://image.auction.co.kr/itemimage/1f/02/25/1f02252172.jpg</t>
-  </si>
-  <si>
-    <t>http://image.auction.co.kr/itemimage/1f/02/25/1f02252173.jpg</t>
-  </si>
-  <si>
-    <t>http://image.auction.co.kr/itemimage/1f/02/25/1f02252174.jpg</t>
+    <t>http://image.auction.co.kr/itemimage/1f/02/25/1f02252136.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -477,6 +298,15 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
@@ -500,18 +330,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="하이퍼링크" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -825,8 +662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52A1471E-8424-B142-A0F3-001C84653003}">
   <dimension ref="A1:E65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="D57" sqref="D57"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -881,7 +718,7 @@
         <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -892,7 +729,7 @@
         <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -903,7 +740,7 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -914,7 +751,7 @@
         <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -925,7 +762,7 @@
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -936,7 +773,7 @@
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -947,7 +784,7 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -958,7 +795,7 @@
         <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -969,7 +806,7 @@
         <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -980,7 +817,7 @@
         <v>26</v>
       </c>
       <c r="C13" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -991,7 +828,7 @@
         <v>27</v>
       </c>
       <c r="C14" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1002,7 +839,7 @@
         <v>28</v>
       </c>
       <c r="C15" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -1013,7 +850,7 @@
         <v>18</v>
       </c>
       <c r="C16" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -1024,7 +861,7 @@
         <v>19</v>
       </c>
       <c r="C17" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -1035,7 +872,7 @@
         <v>7</v>
       </c>
       <c r="C18" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -1046,7 +883,7 @@
         <v>14</v>
       </c>
       <c r="C19" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -1057,7 +894,7 @@
         <v>11</v>
       </c>
       <c r="C20" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -1068,7 +905,7 @@
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -1079,7 +916,7 @@
         <v>10</v>
       </c>
       <c r="C22" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -1090,7 +927,7 @@
         <v>15</v>
       </c>
       <c r="C23" t="s">
-        <v>80</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -1101,7 +938,7 @@
         <v>16</v>
       </c>
       <c r="C24" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -1112,7 +949,7 @@
         <v>29</v>
       </c>
       <c r="C25" t="s">
-        <v>82</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -1123,7 +960,7 @@
         <v>30</v>
       </c>
       <c r="C26" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -1133,8 +970,8 @@
       <c r="B27" t="s">
         <v>21</v>
       </c>
-      <c r="C27" t="s">
-        <v>84</v>
+      <c r="C27" s="1" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -1145,7 +982,7 @@
         <v>32</v>
       </c>
       <c r="C28" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -1156,7 +993,7 @@
         <v>33</v>
       </c>
       <c r="C29" t="s">
-        <v>86</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -1167,7 +1004,7 @@
         <v>34</v>
       </c>
       <c r="C30" t="s">
-        <v>87</v>
+        <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -1178,7 +1015,7 @@
         <v>35</v>
       </c>
       <c r="C31" t="s">
-        <v>88</v>
+        <v>61</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -1189,7 +1026,7 @@
         <v>36</v>
       </c>
       <c r="C32" t="s">
-        <v>89</v>
+        <v>61</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -1200,7 +1037,7 @@
         <v>9</v>
       </c>
       <c r="C33" t="s">
-        <v>90</v>
+        <v>61</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -1211,7 +1048,7 @@
         <v>17</v>
       </c>
       <c r="C34" t="s">
-        <v>91</v>
+        <v>61</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -1222,7 +1059,7 @@
         <v>24</v>
       </c>
       <c r="C35" t="s">
-        <v>92</v>
+        <v>61</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -1233,7 +1070,7 @@
         <v>23</v>
       </c>
       <c r="C36" t="s">
-        <v>93</v>
+        <v>61</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -1244,7 +1081,7 @@
         <v>37</v>
       </c>
       <c r="C37" t="s">
-        <v>94</v>
+        <v>61</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -1255,7 +1092,7 @@
         <v>38</v>
       </c>
       <c r="C38" t="s">
-        <v>95</v>
+        <v>61</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -1266,7 +1103,7 @@
         <v>39</v>
       </c>
       <c r="C39" t="s">
-        <v>96</v>
+        <v>61</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -1277,7 +1114,7 @@
         <v>18</v>
       </c>
       <c r="C40" t="s">
-        <v>97</v>
+        <v>61</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -1288,7 +1125,7 @@
         <v>19</v>
       </c>
       <c r="C41" t="s">
-        <v>98</v>
+        <v>61</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -1299,7 +1136,7 @@
         <v>27</v>
       </c>
       <c r="C42" t="s">
-        <v>99</v>
+        <v>61</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -1310,7 +1147,7 @@
         <v>40</v>
       </c>
       <c r="C43" t="s">
-        <v>100</v>
+        <v>61</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -1321,7 +1158,7 @@
         <v>28</v>
       </c>
       <c r="C44" t="s">
-        <v>101</v>
+        <v>61</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -1332,7 +1169,7 @@
         <v>41</v>
       </c>
       <c r="C45" t="s">
-        <v>102</v>
+        <v>61</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -1343,7 +1180,7 @@
         <v>42</v>
       </c>
       <c r="C46" t="s">
-        <v>103</v>
+        <v>61</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -1354,7 +1191,7 @@
         <v>43</v>
       </c>
       <c r="C47" t="s">
-        <v>104</v>
+        <v>61</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -1365,7 +1202,7 @@
         <v>44</v>
       </c>
       <c r="C48" t="s">
-        <v>105</v>
+        <v>61</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -1376,7 +1213,7 @@
         <v>45</v>
       </c>
       <c r="C49" t="s">
-        <v>106</v>
+        <v>61</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -1387,7 +1224,7 @@
         <v>46</v>
       </c>
       <c r="C50" t="s">
-        <v>107</v>
+        <v>61</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -1398,7 +1235,7 @@
         <v>47</v>
       </c>
       <c r="C51" t="s">
-        <v>108</v>
+        <v>61</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -1409,7 +1246,7 @@
         <v>48</v>
       </c>
       <c r="C52" t="s">
-        <v>109</v>
+        <v>61</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -1420,7 +1257,7 @@
         <v>57</v>
       </c>
       <c r="C53" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -1431,7 +1268,7 @@
         <v>58</v>
       </c>
       <c r="C54" t="s">
-        <v>111</v>
+        <v>61</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -1442,7 +1279,7 @@
         <v>49</v>
       </c>
       <c r="C55" t="s">
-        <v>112</v>
+        <v>61</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -1453,7 +1290,7 @@
         <v>50</v>
       </c>
       <c r="C56" t="s">
-        <v>113</v>
+        <v>61</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -1464,7 +1301,7 @@
         <v>51</v>
       </c>
       <c r="C57" t="s">
-        <v>114</v>
+        <v>61</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -1475,7 +1312,7 @@
         <v>52</v>
       </c>
       <c r="C58" t="s">
-        <v>115</v>
+        <v>61</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -1486,7 +1323,7 @@
         <v>53</v>
       </c>
       <c r="C59" t="s">
-        <v>116</v>
+        <v>61</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -1497,7 +1334,7 @@
         <v>54</v>
       </c>
       <c r="C60" t="s">
-        <v>117</v>
+        <v>61</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -1508,7 +1345,7 @@
         <v>29</v>
       </c>
       <c r="C61" t="s">
-        <v>118</v>
+        <v>61</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -1519,7 +1356,7 @@
         <v>30</v>
       </c>
       <c r="C62" t="s">
-        <v>119</v>
+        <v>61</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -1530,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="C63" t="s">
-        <v>120</v>
+        <v>61</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -1541,7 +1378,7 @@
         <v>55</v>
       </c>
       <c r="C64" t="s">
-        <v>121</v>
+        <v>61</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -1552,11 +1389,14 @@
         <v>56</v>
       </c>
       <c r="C65" t="s">
-        <v>122</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="C27" r:id="rId1" xr:uid="{09558976-C7B9-6942-BA8D-CF617179A46F}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Make Answer Cheking Logic Create a Function that save a data in localstorage Cretae a Funtionn that load localstorage data and get it in any html file
</commit_message>
<xml_diff>
--- a/datafiles/questionDB.xlsx
+++ b/datafiles/questionDB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songi/Desktop/MyProjects/TestMaker/datafiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF46D53E-F886-844B-A767-B15BD8DB64D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E43BF6D-9DD8-0548-8778-E190689F9E40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14400" yWindow="500" windowWidth="14400" windowHeight="17500" xr2:uid="{0D182CA0-F053-8B46-8287-4831F5560F7B}"/>
   </bookViews>
@@ -54,10 +54,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>돼지</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>항정살</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -158,10 +154,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>소</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>윗등심살</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -280,6 +272,14 @@
   </si>
   <si>
     <t>http://image.auction.co.kr/itemimage/1f/02/25/1f02252136.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pig</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cow</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -662,8 +662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52A1471E-8424-B142-A0F3-001C84653003}">
   <dimension ref="A1:E65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -690,706 +690,706 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" t="s">
         <v>5</v>
       </c>
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
       <c r="C9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C14" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="B18" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="B19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C19" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="B20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C20" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="B21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="B22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C22" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="B23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C23" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="B24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C24" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="B25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C25" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="B26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C26" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="B27" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="B28" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C28" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B29" t="s">
         <v>31</v>
       </c>
-      <c r="B29" t="s">
-        <v>33</v>
-      </c>
       <c r="C29" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="B30" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C30" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="B31" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C31" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="B32" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C32" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="B33" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C33" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="B34" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C34" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="B35" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C35" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="B36" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C36" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="B37" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C37" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="B38" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C38" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="B39" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C39" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="B40" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C40" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="B41" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C41" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="B42" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C42" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="B43" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C43" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="B44" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C44" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="B45" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C45" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="B46" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C46" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="B47" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C47" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="B48" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C48" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="B49" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C49" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="B50" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C50" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="B51" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C51" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="B52" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C52" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="B53" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C53" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="B54" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C54" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="B55" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C55" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="B56" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C56" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="B57" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C57" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="B58" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C58" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="B59" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C59" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="B60" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C60" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="B61" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C61" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="B62" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C62" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C63" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C64" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="B65" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C65" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Complete smallpart Test and checking answer Logic Add smallpart quiz DATA BASE to questionDB.xlsx file
Change datamager script to share functons between largepart quiz and smallpart quiz
</commit_message>
<xml_diff>
--- a/datafiles/questionDB.xlsx
+++ b/datafiles/questionDB.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songi/Desktop/MyProjects/TestMaker/datafiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E43BF6D-9DD8-0548-8778-E190689F9E40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EE100FB-70C5-4045-A35A-6CA1A960CBC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="500" windowWidth="14400" windowHeight="17500" xr2:uid="{0D182CA0-F053-8B46-8287-4831F5560F7B}"/>
+    <workbookView xWindow="14400" yWindow="500" windowWidth="14400" windowHeight="17500" activeTab="1" xr2:uid="{0D182CA0-F053-8B46-8287-4831F5560F7B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="largepart" sheetId="1" r:id="rId1"/>
+    <sheet name="smallpart" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="63">
   <si>
     <t>name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -662,8 +663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52A1471E-8424-B142-A0F3-001C84653003}">
   <dimension ref="A1:E65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="C66" sqref="C66"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -1399,4 +1400,150 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA349220-2D7B-DD4A-8D4B-2E9184C5B15F}">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
+  <cols>
+    <col min="3" max="3" width="57.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add Quiz data Image files  change all css style
</commit_message>
<xml_diff>
--- a/datafiles/questionDB.xlsx
+++ b/datafiles/questionDB.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songi/Desktop/MyProjects/TestMaker/datafiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EE100FB-70C5-4045-A35A-6CA1A960CBC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42E07A4C-05A4-314F-8394-4CCA96F4BFF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="500" windowWidth="14400" windowHeight="17500" activeTab="1" xr2:uid="{0D182CA0-F053-8B46-8287-4831F5560F7B}"/>
+    <workbookView xWindow="14400" yWindow="500" windowWidth="14400" windowHeight="17500" xr2:uid="{0D182CA0-F053-8B46-8287-4831F5560F7B}"/>
   </bookViews>
   <sheets>
     <sheet name="largepart" sheetId="1" r:id="rId1"/>
     <sheet name="smallpart" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">largepart!$A$1:$E$65</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="125">
   <si>
     <t>name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -266,21 +269,245 @@
     <t>http://jkmeat.co.kr/skin_shop/standard/s_img/basic/JK-0414_M.jpg</t>
   </si>
   <si>
-    <t>http://www.jkmeat.co.kr/skin_shop/standard/s_img/basic/JK-0424_M.jpg</t>
-  </si>
-  <si>
     <t>http://image.auction.co.kr/itemimage/1f/02/25/1f02252136.jpg</t>
   </si>
   <si>
-    <t>http://image.auction.co.kr/itemimage/1f/02/25/1f02252136.jpg</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>pig</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>cow</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/datafiles/pig/안심살1.png</t>
+  </si>
+  <si>
+    <t>/datafiles/pig/등심살1.png</t>
+  </si>
+  <si>
+    <t>/datafiles/pig/알등심살1.png</t>
+  </si>
+  <si>
+    <t>/datafiles/pig/등심덧살1.png</t>
+  </si>
+  <si>
+    <t>/datafiles/pig/목심살1.png</t>
+  </si>
+  <si>
+    <t>/datafiles/pig/앞다리살1.png</t>
+  </si>
+  <si>
+    <t>/datafiles/pig/앞사태살1.png</t>
+  </si>
+  <si>
+    <t>/datafiles/pig/항정살1.png</t>
+  </si>
+  <si>
+    <t>/datafiles/pig/꾸리살1.png</t>
+  </si>
+  <si>
+    <t>/datafiles/pig/부채살1.png</t>
+  </si>
+  <si>
+    <t>/datafiles/pig/주걱살1.png</t>
+  </si>
+  <si>
+    <t>/datafiles/pig/볼기살1.png</t>
+  </si>
+  <si>
+    <t>/datafiles/pig/설깃살1.png</t>
+  </si>
+  <si>
+    <t>/datafiles/pig/도가니살1.png</t>
+  </si>
+  <si>
+    <t>/datafiles/pig/홍두깨살1.png</t>
+  </si>
+  <si>
+    <t>/datafiles/pig/보섭살1.png</t>
+  </si>
+  <si>
+    <t>/datafiles/pig/뒷사태살1.png</t>
+  </si>
+  <si>
+    <t>/datafiles/pig/삼겹살1.png</t>
+  </si>
+  <si>
+    <t>/datafiles/pig/갈매기살1.png</t>
+  </si>
+  <si>
+    <t>/datafiles/pig/등갈비1.png</t>
+  </si>
+  <si>
+    <t>/datafiles/pig/토시살1.png</t>
+  </si>
+  <si>
+    <t>/datafiles/pig/오돌삼겹1.png</t>
+  </si>
+  <si>
+    <t>/datafiles/pig/갈비1.png</t>
+  </si>
+  <si>
+    <t>/datafiles/pig/갈비살1.png</t>
+  </si>
+  <si>
+    <t>/datafiles/pig/마구리1.png</t>
+  </si>
+  <si>
+    <t>/datafiles/cow/안심살1.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/datafiles/cow/윗등심살1.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/datafiles/cow/꽃등심살1.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/datafiles/cow/아래등심살1.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/datafiles/cow/살치살1.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/datafiles/cow/채끝살1.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/datafiles/cow/목심살1.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/datafiles/cow/꾸리살1.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/datafiles/cow/부채살1.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/datafiles/cow/앞다리살1.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/datafiles/cow/갈비덧살1.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/datafiles/cow/부채덮개살1.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/datafiles/cow/우둔살1.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/datafiles/cow/홍두깨살1.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/datafiles/cow/보섭살1.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/datafiles/cow/설깃살1.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/datafiles/cow/설깃머리살1.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/datafiles/cow/도가니살1.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/datafiles/cow/삼각살1.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/datafiles/cow/양지머리1.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/datafiles/cow/차돌박이1.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/datafiles/cow/업진살1.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/datafiles/cow/업진안살1.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/datafiles/cow/치마양지1.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/datafiles/cow/치마살1.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/datafiles/cow/앞치마살1.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/datafiles/cow/앞사태1.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/datafiles/cow/뒷사태1.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/datafiles/cow/뭉치사태1.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/datafiles/cow/아롱사태1.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/datafiles/cow/상박살1.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/datafiles/cow/본갈비1.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/datafiles/cow/꽃갈비1.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/datafiles/cow/참갈비1.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/datafiles/cow/갈비살1.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/datafiles/cow/마구리1.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/datafiles/cow/토시살1.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/datafiles/cow/안창살1.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/datafiles/cow/제비추리1.png</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -288,7 +515,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -299,15 +526,6 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="맑은 고딕"/>
-      <family val="2"/>
-      <charset val="129"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
       <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
@@ -331,25 +549,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
-    <cellStyle name="하이퍼링크" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -663,8 +874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52A1471E-8424-B142-A0F3-001C84653003}">
   <dimension ref="A1:E65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -691,713 +902,710 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B2" t="s">
         <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B5" t="s">
         <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B7" t="s">
         <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B10" t="s">
         <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B11" t="s">
         <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B12" t="s">
         <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B13" t="s">
         <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B14" t="s">
         <v>26</v>
       </c>
       <c r="C14" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B15" t="s">
         <v>27</v>
       </c>
       <c r="C15" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B16" t="s">
         <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B17" t="s">
         <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B18" t="s">
         <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B19" t="s">
         <v>13</v>
       </c>
       <c r="C19" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B20" t="s">
         <v>10</v>
       </c>
       <c r="C20" t="s">
-        <v>58</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B21" t="s">
         <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B22" t="s">
         <v>9</v>
       </c>
       <c r="C22" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B23" t="s">
         <v>14</v>
       </c>
       <c r="C23" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B24" t="s">
         <v>15</v>
       </c>
       <c r="C24" t="s">
-        <v>58</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B25" t="s">
         <v>28</v>
       </c>
       <c r="C25" t="s">
-        <v>58</v>
+        <v>84</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B26" t="s">
         <v>29</v>
       </c>
       <c r="C26" t="s">
-        <v>58</v>
+        <v>85</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B27" t="s">
         <v>20</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>60</v>
+      <c r="C27" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B28" t="s">
         <v>30</v>
       </c>
       <c r="C28" t="s">
-        <v>59</v>
+        <v>87</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B29" t="s">
         <v>31</v>
       </c>
       <c r="C29" t="s">
-        <v>59</v>
+        <v>88</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B30" t="s">
         <v>32</v>
       </c>
       <c r="C30" t="s">
-        <v>59</v>
+        <v>89</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B31" t="s">
         <v>33</v>
       </c>
       <c r="C31" t="s">
-        <v>59</v>
+        <v>90</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B32" t="s">
         <v>34</v>
       </c>
       <c r="C32" t="s">
-        <v>59</v>
+        <v>91</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B33" t="s">
         <v>8</v>
       </c>
       <c r="C33" t="s">
-        <v>59</v>
+        <v>92</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B34" t="s">
         <v>16</v>
       </c>
       <c r="C34" t="s">
-        <v>59</v>
+        <v>93</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B35" t="s">
         <v>23</v>
       </c>
       <c r="C35" t="s">
-        <v>59</v>
+        <v>94</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B36" t="s">
         <v>22</v>
       </c>
       <c r="C36" t="s">
-        <v>59</v>
+        <v>95</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B37" t="s">
         <v>35</v>
       </c>
       <c r="C37" t="s">
-        <v>59</v>
+        <v>96</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B38" t="s">
         <v>36</v>
       </c>
       <c r="C38" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B39" t="s">
         <v>37</v>
       </c>
       <c r="C39" t="s">
-        <v>59</v>
+        <v>98</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B40" t="s">
         <v>17</v>
       </c>
       <c r="C40" t="s">
-        <v>59</v>
+        <v>99</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B41" t="s">
         <v>18</v>
       </c>
       <c r="C41" t="s">
-        <v>59</v>
+        <v>100</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B42" t="s">
         <v>26</v>
       </c>
       <c r="C42" t="s">
-        <v>59</v>
+        <v>101</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B43" t="s">
         <v>38</v>
       </c>
       <c r="C43" t="s">
-        <v>59</v>
+        <v>102</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B44" t="s">
         <v>27</v>
       </c>
       <c r="C44" t="s">
-        <v>59</v>
+        <v>103</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B45" t="s">
         <v>39</v>
       </c>
       <c r="C45" t="s">
-        <v>59</v>
+        <v>104</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B46" t="s">
         <v>40</v>
       </c>
       <c r="C46" t="s">
-        <v>59</v>
+        <v>105</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B47" t="s">
         <v>41</v>
       </c>
       <c r="C47" t="s">
-        <v>59</v>
+        <v>106</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B48" t="s">
         <v>42</v>
       </c>
       <c r="C48" t="s">
-        <v>59</v>
+        <v>107</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B49" t="s">
         <v>43</v>
       </c>
       <c r="C49" t="s">
-        <v>59</v>
+        <v>108</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B50" t="s">
         <v>44</v>
       </c>
       <c r="C50" t="s">
-        <v>59</v>
+        <v>109</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B51" t="s">
         <v>45</v>
       </c>
       <c r="C51" t="s">
-        <v>59</v>
+        <v>110</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B52" t="s">
         <v>46</v>
       </c>
       <c r="C52" t="s">
-        <v>59</v>
+        <v>111</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B53" t="s">
         <v>55</v>
       </c>
       <c r="C53" t="s">
-        <v>59</v>
+        <v>112</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B54" t="s">
         <v>56</v>
       </c>
       <c r="C54" t="s">
-        <v>59</v>
+        <v>113</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B55" t="s">
         <v>47</v>
       </c>
       <c r="C55" t="s">
-        <v>59</v>
+        <v>114</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B56" t="s">
         <v>48</v>
       </c>
       <c r="C56" t="s">
-        <v>59</v>
+        <v>115</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B57" t="s">
         <v>49</v>
       </c>
       <c r="C57" t="s">
-        <v>59</v>
+        <v>116</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B58" t="s">
         <v>50</v>
       </c>
       <c r="C58" t="s">
-        <v>59</v>
+        <v>117</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B59" t="s">
         <v>51</v>
       </c>
       <c r="C59" t="s">
-        <v>59</v>
+        <v>118</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B60" t="s">
         <v>52</v>
       </c>
       <c r="C60" t="s">
-        <v>59</v>
+        <v>119</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B61" t="s">
         <v>28</v>
       </c>
       <c r="C61" t="s">
-        <v>59</v>
+        <v>120</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B62" t="s">
         <v>29</v>
       </c>
       <c r="C62" t="s">
-        <v>59</v>
+        <v>121</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B63" t="s">
         <v>9</v>
       </c>
       <c r="C63" t="s">
-        <v>59</v>
+        <v>122</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B64" t="s">
         <v>53</v>
       </c>
       <c r="C64" t="s">
-        <v>59</v>
+        <v>123</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B65" t="s">
         <v>54</v>
       </c>
       <c r="C65" t="s">
-        <v>59</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="C27" r:id="rId1" xr:uid="{09558976-C7B9-6942-BA8D-CF617179A46F}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1406,7 +1614,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA349220-2D7B-DD4A-8D4B-2E9184C5B15F}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -1434,7 +1642,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B2" t="s">
         <v>27</v>
@@ -1445,7 +1653,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B3" t="s">
         <v>23</v>
@@ -1456,7 +1664,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s">
         <v>26</v>
@@ -1467,7 +1675,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
@@ -1478,7 +1686,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
@@ -1489,57 +1697,57 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B7" t="s">
         <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B8" t="s">
         <v>48</v>
       </c>
       <c r="C8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B9" t="s">
         <v>39</v>
       </c>
       <c r="C9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B10" t="s">
         <v>54</v>
       </c>
       <c r="C10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B11" t="s">
         <v>42</v>
       </c>
       <c r="C11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change local file path / -> ./
</commit_message>
<xml_diff>
--- a/datafiles/questionDB.xlsx
+++ b/datafiles/questionDB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songi/Desktop/MyProjects/TestMaker/datafiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42E07A4C-05A4-314F-8394-4CCA96F4BFF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70CDF7DD-AAF1-BD4A-8A43-C9F0F3E5AE36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14400" yWindow="500" windowWidth="14400" windowHeight="17500" xr2:uid="{0D182CA0-F053-8B46-8287-4831F5560F7B}"/>
   </bookViews>
@@ -280,235 +280,196 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>/datafiles/pig/안심살1.png</t>
-  </si>
-  <si>
-    <t>/datafiles/pig/등심살1.png</t>
-  </si>
-  <si>
-    <t>/datafiles/pig/알등심살1.png</t>
-  </si>
-  <si>
-    <t>/datafiles/pig/등심덧살1.png</t>
-  </si>
-  <si>
-    <t>/datafiles/pig/목심살1.png</t>
-  </si>
-  <si>
-    <t>/datafiles/pig/앞다리살1.png</t>
-  </si>
-  <si>
-    <t>/datafiles/pig/앞사태살1.png</t>
-  </si>
-  <si>
-    <t>/datafiles/pig/항정살1.png</t>
-  </si>
-  <si>
-    <t>/datafiles/pig/꾸리살1.png</t>
-  </si>
-  <si>
-    <t>/datafiles/pig/부채살1.png</t>
-  </si>
-  <si>
-    <t>/datafiles/pig/주걱살1.png</t>
-  </si>
-  <si>
-    <t>/datafiles/pig/볼기살1.png</t>
-  </si>
-  <si>
-    <t>/datafiles/pig/설깃살1.png</t>
-  </si>
-  <si>
-    <t>/datafiles/pig/도가니살1.png</t>
-  </si>
-  <si>
-    <t>/datafiles/pig/홍두깨살1.png</t>
-  </si>
-  <si>
-    <t>/datafiles/pig/보섭살1.png</t>
-  </si>
-  <si>
-    <t>/datafiles/pig/뒷사태살1.png</t>
-  </si>
-  <si>
-    <t>/datafiles/pig/삼겹살1.png</t>
-  </si>
-  <si>
-    <t>/datafiles/pig/갈매기살1.png</t>
-  </si>
-  <si>
-    <t>/datafiles/pig/등갈비1.png</t>
-  </si>
-  <si>
-    <t>/datafiles/pig/토시살1.png</t>
-  </si>
-  <si>
-    <t>/datafiles/pig/오돌삼겹1.png</t>
-  </si>
-  <si>
-    <t>/datafiles/pig/갈비1.png</t>
-  </si>
-  <si>
-    <t>/datafiles/pig/갈비살1.png</t>
-  </si>
-  <si>
-    <t>/datafiles/pig/마구리1.png</t>
-  </si>
-  <si>
-    <t>/datafiles/cow/안심살1.png</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/datafiles/cow/윗등심살1.png</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/datafiles/cow/꽃등심살1.png</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/datafiles/cow/아래등심살1.png</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/datafiles/cow/살치살1.png</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/datafiles/cow/채끝살1.png</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/datafiles/cow/목심살1.png</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/datafiles/cow/꾸리살1.png</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/datafiles/cow/부채살1.png</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/datafiles/cow/앞다리살1.png</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/datafiles/cow/갈비덧살1.png</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/datafiles/cow/부채덮개살1.png</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/datafiles/cow/우둔살1.png</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/datafiles/cow/홍두깨살1.png</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/datafiles/cow/보섭살1.png</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/datafiles/cow/설깃살1.png</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/datafiles/cow/설깃머리살1.png</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/datafiles/cow/도가니살1.png</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/datafiles/cow/삼각살1.png</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/datafiles/cow/양지머리1.png</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/datafiles/cow/차돌박이1.png</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/datafiles/cow/업진살1.png</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/datafiles/cow/업진안살1.png</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/datafiles/cow/치마양지1.png</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/datafiles/cow/치마살1.png</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/datafiles/cow/앞치마살1.png</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/datafiles/cow/앞사태1.png</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/datafiles/cow/뒷사태1.png</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/datafiles/cow/뭉치사태1.png</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/datafiles/cow/아롱사태1.png</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/datafiles/cow/상박살1.png</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/datafiles/cow/본갈비1.png</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/datafiles/cow/꽃갈비1.png</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/datafiles/cow/참갈비1.png</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/datafiles/cow/갈비살1.png</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/datafiles/cow/마구리1.png</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/datafiles/cow/토시살1.png</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/datafiles/cow/안창살1.png</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/datafiles/cow/제비추리1.png</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>./datafiles/pig/안심살1.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/등심살1.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/알등심살1.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/등심덧살1.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/목심살1.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/앞다리살1.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/앞사태살1.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/항정살1.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/꾸리살1.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/부채살1.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/주걱살1.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/볼기살1.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/설깃살1.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/도가니살1.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/홍두깨살1.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/보섭살1.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/뒷사태살1.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/삼겹살1.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/갈매기살1.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/등갈비1.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/토시살1.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/오돌삼겹1.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/갈비1.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/갈비살1.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/마구리1.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/안심살1.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/윗등심살1.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/꽃등심살1.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/아래등심살1.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/살치살1.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/채끝살1.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/목심살1.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/꾸리살1.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/부채살1.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/앞다리살1.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/갈비덧살1.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/부채덮개살1.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/우둔살1.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/홍두깨살1.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/보섭살1.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/설깃살1.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/설깃머리살1.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/도가니살1.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/삼각살1.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/양지머리1.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/차돌박이1.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/업진살1.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/업진안살1.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/치마양지1.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/치마살1.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/앞치마살1.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/앞사태1.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/뒷사태1.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/뭉치사태1.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/아롱사태1.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/상박살1.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/본갈비1.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/꽃갈비1.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/참갈비1.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/갈비살1.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/마구리1.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/토시살1.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/안창살1.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/제비추리1.png</t>
   </si>
 </sst>
 </file>
@@ -874,8 +835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52A1471E-8424-B142-A0F3-001C84653003}">
   <dimension ref="A1:E65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>

</xml_diff>

<commit_message>
Add Quiz Image files
</commit_message>
<xml_diff>
--- a/datafiles/questionDB.xlsx
+++ b/datafiles/questionDB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songi/Desktop/MyProjects/TestMaker/datafiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70CDF7DD-AAF1-BD4A-8A43-C9F0F3E5AE36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE7FA4A4-50AB-C94E-8C89-86D6C1974CC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="500" windowWidth="14400" windowHeight="17500" xr2:uid="{0D182CA0-F053-8B46-8287-4831F5560F7B}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{0D182CA0-F053-8B46-8287-4831F5560F7B}"/>
   </bookViews>
   <sheets>
     <sheet name="largepart" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="261">
   <si>
     <t>name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -266,12 +266,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>http://jkmeat.co.kr/skin_shop/standard/s_img/basic/JK-0414_M.jpg</t>
-  </si>
-  <si>
-    <t>http://image.auction.co.kr/itemimage/1f/02/25/1f02252136.jpg</t>
-  </si>
-  <si>
     <t>pig</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -470,13 +464,437 @@
   </si>
   <si>
     <t>./datafiles/cow/제비추리1.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/안심살2.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/안심살3.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/등심살2.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/등심살3.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/알등심살2.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/알등심살3.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/등심덧살2.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/등심덧살3.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/목심살2.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/목심살3.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/앞다리살2.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/앞다리살3.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/앞사태살2.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/앞사태살3.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/항정살2.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/항정살3.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/꾸리살2.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/꾸리살3.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/부채살2.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/부채살3.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/주걱살2.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/주걱살3.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/볼기살2.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/볼기살3.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/설깃살2.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/설깃살3.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/도가니살2.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/도가니살3.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/홍두깨살2.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/홍두깨살3.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/보섭살2.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/보섭살3.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/뒷사태살2.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/뒷사태살3.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/삼겹살2.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/삼겹살3.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/갈매기살2.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/갈매기살3.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/등갈비2.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/등갈비3.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/토시살2.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/토시살3.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/오돌삼겹2.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/오돌삼겹3.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/갈비2.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/갈비3.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/갈비살2.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/갈비살3.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/마구리2.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/마구리3.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/안심살2.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/안심살3.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/윗등심살2.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/윗등심살3.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/꽃등심살2.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/꽃등심살3.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/아래등심살2.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/아래등심살3.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/살치살2.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/살치살3.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/채끝살2.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/채끝살3.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/목심살2.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/목심살3.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/꾸리살2.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/꾸리살3.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/부채살2.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/부채살3.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/앞다리살2.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/앞다리살3.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/갈비덧살2.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/갈비덧살3.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/부채덮개살2.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/부채덮개살3.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/우둔살2.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/우둔살3.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/홍두깨살2.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/홍두깨살3.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/보섭살2.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/보섭살3.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/설깃살2.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/설깃살3.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/설깃머리살2.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/설깃머리살3.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/도가니살2.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/도가니살3.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/삼각살2.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/삼각살3.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/양지머리2.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/양지머리3.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/차돌박이2.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/차돌박이3.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/업진살2.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/업진살3.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/업진안살2.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/업진안살3.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/치마양지2.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/치마양지3.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/치마살2.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/치마살3.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/앞치마살2.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/앞치마살3.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/앞사태2.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/앞사태3.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/뒷사태2.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/뒷사태3.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/뭉치사태2.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/뭉치사태3.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/아롱사태2.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/아롱사태3.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/상박살2.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/상박살3.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/본갈비2.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/본갈비3.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/꽃갈비2.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/꽃갈비3.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/참갈비2.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/참갈비3.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/갈비살2.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/갈비살3.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/마구리2.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/마구리3.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/토시살2.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/토시살3.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/안창살2.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/안창살3.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/제비추리2.png</t>
+  </si>
+  <si>
+    <t>./datafiles/cow/제비추리3.png</t>
+  </si>
+  <si>
+    <t>./datafiles/pig/도가니살1.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>./datafiles/pig/부채살1.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>./datafiles/pig/설깃살1.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>./datafiles/pig/항정살1.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>./datafiles/pig/목심살1.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>./datafiles/cow/채끝살1.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>./datafiles/cow/아롱사태1.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>./datafiles/cow/삼각살1.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>./datafiles/cow/제비추리1.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>./datafiles/cow/업진살1.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -487,6 +905,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
@@ -515,8 +941,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -835,13 +1264,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52A1471E-8424-B142-A0F3-001C84653003}">
   <dimension ref="A1:E65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
   <cols>
-    <col min="3" max="3" width="57.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -863,706 +1292,1090 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
         <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>61</v>
+        <v>59</v>
+      </c>
+      <c r="D2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E2" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>62</v>
+        <v>60</v>
+      </c>
+      <c r="D3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E3" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>63</v>
+        <v>61</v>
+      </c>
+      <c r="D4" t="s">
+        <v>127</v>
+      </c>
+      <c r="E4" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B5" t="s">
         <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>64</v>
+        <v>62</v>
+      </c>
+      <c r="D5" t="s">
+        <v>129</v>
+      </c>
+      <c r="E5" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>65</v>
+        <v>63</v>
+      </c>
+      <c r="D6" t="s">
+        <v>131</v>
+      </c>
+      <c r="E6" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B7" t="s">
         <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>66</v>
+        <v>64</v>
+      </c>
+      <c r="D7" t="s">
+        <v>133</v>
+      </c>
+      <c r="E7" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>67</v>
+        <v>65</v>
+      </c>
+      <c r="D8" t="s">
+        <v>135</v>
+      </c>
+      <c r="E8" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>68</v>
+        <v>66</v>
+      </c>
+      <c r="D9" t="s">
+        <v>137</v>
+      </c>
+      <c r="E9" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B10" t="s">
         <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>69</v>
+        <v>67</v>
+      </c>
+      <c r="D10" t="s">
+        <v>139</v>
+      </c>
+      <c r="E10" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B11" t="s">
         <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>70</v>
+        <v>68</v>
+      </c>
+      <c r="D11" t="s">
+        <v>141</v>
+      </c>
+      <c r="E11" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B12" t="s">
         <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>71</v>
+        <v>69</v>
+      </c>
+      <c r="D12" t="s">
+        <v>143</v>
+      </c>
+      <c r="E12" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B13" t="s">
         <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>72</v>
+        <v>70</v>
+      </c>
+      <c r="D13" t="s">
+        <v>145</v>
+      </c>
+      <c r="E13" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B14" t="s">
         <v>26</v>
       </c>
       <c r="C14" t="s">
-        <v>73</v>
+        <v>71</v>
+      </c>
+      <c r="D14" t="s">
+        <v>147</v>
+      </c>
+      <c r="E14" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B15" t="s">
         <v>27</v>
       </c>
       <c r="C15" t="s">
-        <v>74</v>
+        <v>72</v>
+      </c>
+      <c r="D15" t="s">
+        <v>149</v>
+      </c>
+      <c r="E15" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B16" t="s">
         <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+        <v>73</v>
+      </c>
+      <c r="D16" t="s">
+        <v>151</v>
+      </c>
+      <c r="E16" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B17" t="s">
         <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+        <v>74</v>
+      </c>
+      <c r="D17" t="s">
+        <v>153</v>
+      </c>
+      <c r="E17" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B18" t="s">
         <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+        <v>75</v>
+      </c>
+      <c r="D18" t="s">
+        <v>155</v>
+      </c>
+      <c r="E18" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B19" t="s">
         <v>13</v>
       </c>
       <c r="C19" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
+        <v>76</v>
+      </c>
+      <c r="D19" t="s">
+        <v>157</v>
+      </c>
+      <c r="E19" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B20" t="s">
         <v>10</v>
       </c>
       <c r="C20" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
+        <v>77</v>
+      </c>
+      <c r="D20" t="s">
+        <v>159</v>
+      </c>
+      <c r="E20" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B21" t="s">
         <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
+        <v>78</v>
+      </c>
+      <c r="D21" t="s">
+        <v>161</v>
+      </c>
+      <c r="E21" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B22" t="s">
         <v>9</v>
       </c>
       <c r="C22" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
+        <v>79</v>
+      </c>
+      <c r="D22" t="s">
+        <v>163</v>
+      </c>
+      <c r="E22" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B23" t="s">
         <v>14</v>
       </c>
       <c r="C23" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
+        <v>80</v>
+      </c>
+      <c r="D23" t="s">
+        <v>165</v>
+      </c>
+      <c r="E23" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B24" t="s">
         <v>15</v>
       </c>
       <c r="C24" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
+        <v>81</v>
+      </c>
+      <c r="D24" t="s">
+        <v>167</v>
+      </c>
+      <c r="E24" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B25" t="s">
         <v>28</v>
       </c>
       <c r="C25" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
+        <v>82</v>
+      </c>
+      <c r="D25" t="s">
+        <v>169</v>
+      </c>
+      <c r="E25" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B26" t="s">
         <v>29</v>
       </c>
       <c r="C26" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
+        <v>83</v>
+      </c>
+      <c r="D26" t="s">
+        <v>171</v>
+      </c>
+      <c r="E26" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B27" t="s">
         <v>20</v>
       </c>
       <c r="C27" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
+        <v>84</v>
+      </c>
+      <c r="D27" t="s">
+        <v>173</v>
+      </c>
+      <c r="E27" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B28" t="s">
         <v>30</v>
       </c>
       <c r="C28" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
+        <v>85</v>
+      </c>
+      <c r="D28" t="s">
+        <v>175</v>
+      </c>
+      <c r="E28" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B29" t="s">
         <v>31</v>
       </c>
       <c r="C29" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
+        <v>86</v>
+      </c>
+      <c r="D29" t="s">
+        <v>177</v>
+      </c>
+      <c r="E29" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B30" t="s">
         <v>32</v>
       </c>
       <c r="C30" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
+        <v>87</v>
+      </c>
+      <c r="D30" t="s">
+        <v>179</v>
+      </c>
+      <c r="E30" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B31" t="s">
         <v>33</v>
       </c>
       <c r="C31" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
+        <v>88</v>
+      </c>
+      <c r="D31" t="s">
+        <v>181</v>
+      </c>
+      <c r="E31" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="A32" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B32" t="s">
         <v>34</v>
       </c>
       <c r="C32" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
+        <v>89</v>
+      </c>
+      <c r="D32" t="s">
+        <v>183</v>
+      </c>
+      <c r="E32" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B33" t="s">
         <v>8</v>
       </c>
       <c r="C33" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
+        <v>90</v>
+      </c>
+      <c r="D33" t="s">
+        <v>185</v>
+      </c>
+      <c r="E33" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B34" t="s">
         <v>16</v>
       </c>
       <c r="C34" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
+        <v>91</v>
+      </c>
+      <c r="D34" t="s">
+        <v>187</v>
+      </c>
+      <c r="E34" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
       <c r="A35" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B35" t="s">
         <v>23</v>
       </c>
       <c r="C35" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
+        <v>92</v>
+      </c>
+      <c r="D35" t="s">
+        <v>189</v>
+      </c>
+      <c r="E35" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B36" t="s">
         <v>22</v>
       </c>
       <c r="C36" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
+        <v>93</v>
+      </c>
+      <c r="D36" t="s">
+        <v>191</v>
+      </c>
+      <c r="E36" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
       <c r="A37" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B37" t="s">
         <v>35</v>
       </c>
       <c r="C37" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
+        <v>94</v>
+      </c>
+      <c r="D37" t="s">
+        <v>193</v>
+      </c>
+      <c r="E37" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
       <c r="A38" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B38" t="s">
         <v>36</v>
       </c>
       <c r="C38" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
+        <v>95</v>
+      </c>
+      <c r="D38" t="s">
+        <v>195</v>
+      </c>
+      <c r="E38" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
       <c r="A39" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B39" t="s">
         <v>37</v>
       </c>
       <c r="C39" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
+        <v>96</v>
+      </c>
+      <c r="D39" t="s">
+        <v>197</v>
+      </c>
+      <c r="E39" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
       <c r="A40" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B40" t="s">
         <v>17</v>
       </c>
       <c r="C40" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
+        <v>97</v>
+      </c>
+      <c r="D40" t="s">
+        <v>199</v>
+      </c>
+      <c r="E40" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
       <c r="A41" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B41" t="s">
         <v>18</v>
       </c>
       <c r="C41" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
+        <v>98</v>
+      </c>
+      <c r="D41" t="s">
+        <v>201</v>
+      </c>
+      <c r="E41" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
       <c r="A42" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B42" t="s">
         <v>26</v>
       </c>
       <c r="C42" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
+        <v>99</v>
+      </c>
+      <c r="D42" t="s">
+        <v>203</v>
+      </c>
+      <c r="E42" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
       <c r="A43" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B43" t="s">
         <v>38</v>
       </c>
       <c r="C43" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
+        <v>100</v>
+      </c>
+      <c r="D43" t="s">
+        <v>205</v>
+      </c>
+      <c r="E43" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
       <c r="A44" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B44" t="s">
         <v>27</v>
       </c>
       <c r="C44" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
+        <v>101</v>
+      </c>
+      <c r="D44" t="s">
+        <v>207</v>
+      </c>
+      <c r="E44" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
       <c r="A45" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B45" t="s">
         <v>39</v>
       </c>
       <c r="C45" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
+        <v>102</v>
+      </c>
+      <c r="D45" t="s">
+        <v>209</v>
+      </c>
+      <c r="E45" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
       <c r="A46" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B46" t="s">
         <v>40</v>
       </c>
       <c r="C46" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
+        <v>103</v>
+      </c>
+      <c r="D46" t="s">
+        <v>211</v>
+      </c>
+      <c r="E46" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
       <c r="A47" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B47" t="s">
         <v>41</v>
       </c>
       <c r="C47" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
+        <v>104</v>
+      </c>
+      <c r="D47" t="s">
+        <v>213</v>
+      </c>
+      <c r="E47" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
       <c r="A48" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B48" t="s">
         <v>42</v>
       </c>
       <c r="C48" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
+        <v>105</v>
+      </c>
+      <c r="D48" t="s">
+        <v>215</v>
+      </c>
+      <c r="E48" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
       <c r="A49" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B49" t="s">
         <v>43</v>
       </c>
       <c r="C49" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
+        <v>106</v>
+      </c>
+      <c r="D49" t="s">
+        <v>217</v>
+      </c>
+      <c r="E49" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
       <c r="A50" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B50" t="s">
         <v>44</v>
       </c>
       <c r="C50" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3">
+        <v>107</v>
+      </c>
+      <c r="D50" t="s">
+        <v>219</v>
+      </c>
+      <c r="E50" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
       <c r="A51" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B51" t="s">
         <v>45</v>
       </c>
       <c r="C51" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
+        <v>108</v>
+      </c>
+      <c r="D51" t="s">
+        <v>221</v>
+      </c>
+      <c r="E51" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
       <c r="A52" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B52" t="s">
         <v>46</v>
       </c>
       <c r="C52" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3">
+        <v>109</v>
+      </c>
+      <c r="D52" t="s">
+        <v>223</v>
+      </c>
+      <c r="E52" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
       <c r="A53" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B53" t="s">
         <v>55</v>
       </c>
       <c r="C53" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3">
+        <v>110</v>
+      </c>
+      <c r="D53" t="s">
+        <v>225</v>
+      </c>
+      <c r="E53" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
       <c r="A54" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B54" t="s">
         <v>56</v>
       </c>
       <c r="C54" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3">
+        <v>111</v>
+      </c>
+      <c r="D54" t="s">
+        <v>227</v>
+      </c>
+      <c r="E54" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
       <c r="A55" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B55" t="s">
         <v>47</v>
       </c>
       <c r="C55" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3">
+        <v>112</v>
+      </c>
+      <c r="D55" t="s">
+        <v>229</v>
+      </c>
+      <c r="E55" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
       <c r="A56" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B56" t="s">
         <v>48</v>
       </c>
       <c r="C56" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3">
+        <v>113</v>
+      </c>
+      <c r="D56" t="s">
+        <v>231</v>
+      </c>
+      <c r="E56" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
       <c r="A57" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B57" t="s">
         <v>49</v>
       </c>
       <c r="C57" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3">
+        <v>114</v>
+      </c>
+      <c r="D57" t="s">
+        <v>233</v>
+      </c>
+      <c r="E57" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
       <c r="A58" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B58" t="s">
         <v>50</v>
       </c>
       <c r="C58" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3">
+        <v>115</v>
+      </c>
+      <c r="D58" t="s">
+        <v>235</v>
+      </c>
+      <c r="E58" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
       <c r="A59" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B59" t="s">
         <v>51</v>
       </c>
       <c r="C59" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3">
+        <v>116</v>
+      </c>
+      <c r="D59" t="s">
+        <v>237</v>
+      </c>
+      <c r="E59" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
       <c r="A60" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B60" t="s">
         <v>52</v>
       </c>
       <c r="C60" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
+        <v>117</v>
+      </c>
+      <c r="D60" t="s">
+        <v>239</v>
+      </c>
+      <c r="E60" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
       <c r="A61" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B61" t="s">
         <v>28</v>
       </c>
       <c r="C61" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3">
+        <v>118</v>
+      </c>
+      <c r="D61" t="s">
+        <v>241</v>
+      </c>
+      <c r="E61" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
       <c r="A62" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B62" t="s">
         <v>29</v>
       </c>
       <c r="C62" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3">
+        <v>119</v>
+      </c>
+      <c r="D62" t="s">
+        <v>243</v>
+      </c>
+      <c r="E62" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
       <c r="A63" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B63" t="s">
         <v>9</v>
       </c>
       <c r="C63" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3">
+        <v>120</v>
+      </c>
+      <c r="D63" t="s">
+        <v>245</v>
+      </c>
+      <c r="E63" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
       <c r="A64" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B64" t="s">
         <v>53</v>
       </c>
       <c r="C64" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3">
+        <v>121</v>
+      </c>
+      <c r="D64" t="s">
+        <v>247</v>
+      </c>
+      <c r="E64" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
       <c r="A65" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B65" t="s">
         <v>54</v>
       </c>
       <c r="C65" t="s">
-        <v>124</v>
+        <v>122</v>
+      </c>
+      <c r="D65" t="s">
+        <v>249</v>
+      </c>
+      <c r="E65" t="s">
+        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -1575,13 +2388,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA349220-2D7B-DD4A-8D4B-2E9184C5B15F}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
   <cols>
-    <col min="3" max="3" width="57.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="26.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1603,112 +2416,172 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
         <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
+        <v>251</v>
+      </c>
+      <c r="D2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E2" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s">
         <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>57</v>
+        <v>252</v>
+      </c>
+      <c r="D3" t="s">
+        <v>141</v>
+      </c>
+      <c r="E3" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B4" t="s">
         <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>57</v>
+        <v>253</v>
+      </c>
+      <c r="D4" t="s">
+        <v>147</v>
+      </c>
+      <c r="E4" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>57</v>
+        <v>254</v>
+      </c>
+      <c r="D5" t="s">
+        <v>137</v>
+      </c>
+      <c r="E5" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>57</v>
+        <v>255</v>
+      </c>
+      <c r="D6" t="s">
+        <v>131</v>
+      </c>
+      <c r="E6" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B7" t="s">
         <v>34</v>
       </c>
-      <c r="C7" t="s">
-        <v>58</v>
+      <c r="C7" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B8" t="s">
         <v>48</v>
       </c>
-      <c r="C8" t="s">
-        <v>58</v>
+      <c r="C8" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B9" t="s">
         <v>39</v>
       </c>
-      <c r="C9" t="s">
-        <v>58</v>
+      <c r="C9" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B10" t="s">
         <v>54</v>
       </c>
-      <c r="C10" t="s">
-        <v>58</v>
+      <c r="C10" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
         <v>42</v>
       </c>
-      <c r="C11" t="s">
-        <v>58</v>
+      <c r="C11" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>216</v>
       </c>
     </row>
   </sheetData>

</xml_diff>